<commit_message>
fix: Resolved the issue of extra blank spaces of removed paragraphs
</commit_message>
<xml_diff>
--- a/resources/section_mapping.xlsx
+++ b/resources/section_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="11570" tabRatio="453" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="11570" tabRatio="453"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1108,7 +1108,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -2712,7 +2712,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improvements in CHECKBOX and RADIO questions
* Refactored the logic to handle the RADIO questions.
** Fixed the bug of overwriting due to repeated keys ('yes'/'no')
* Started the implementation for ##NONE# type of answers: Accept similar
values also (viz. no, blank, etc.)
</commit_message>
<xml_diff>
--- a/resources/section_mapping.xlsx
+++ b/resources/section_mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satyesha\PycharmProjects\application_questionnaire\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DEV\PycharmProjects\application_questionnaire\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="11570" tabRatio="453"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11565" tabRatio="453"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="205">
   <si>
     <t>Sections</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>4.4.1</t>
@@ -650,12 +647,15 @@
   <si>
     <t>&lt;&lt;$File and Registry Permissions&gt;&gt;</t>
   </si>
+  <si>
+    <t>##NONE##</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,13 +673,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -757,7 +750,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,48 +1058,48 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="48" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>385</v>
       </c>
@@ -1118,16 +1111,16 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>386</v>
       </c>
@@ -1135,22 +1128,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="3">
         <v>4.2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>386</v>
       </c>
@@ -1158,20 +1151,20 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>386</v>
       </c>
@@ -1185,14 +1178,14 @@
         <v>33</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>386</v>
       </c>
@@ -1206,14 +1199,14 @@
         <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>386</v>
       </c>
@@ -1227,14 +1220,14 @@
         <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>386</v>
       </c>
@@ -1248,14 +1241,14 @@
         <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>386</v>
       </c>
@@ -1269,14 +1262,14 @@
         <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>386</v>
       </c>
@@ -1290,14 +1283,14 @@
         <v>38</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>386</v>
       </c>
@@ -1311,14 +1304,14 @@
         <v>39</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>386</v>
       </c>
@@ -1332,14 +1325,14 @@
         <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>386</v>
       </c>
@@ -1353,14 +1346,14 @@
         <v>41</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>386</v>
       </c>
@@ -1374,14 +1367,14 @@
         <v>42</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>387</v>
       </c>
@@ -1389,20 +1382,20 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>388</v>
       </c>
@@ -1410,22 +1403,22 @@
         <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D16" s="3">
         <v>4.3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>388</v>
       </c>
@@ -1439,14 +1432,14 @@
         <v>49</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>388</v>
       </c>
@@ -1460,14 +1453,14 @@
         <v>50</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>388</v>
       </c>
@@ -1481,14 +1474,14 @@
         <v>51</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>388</v>
       </c>
@@ -1502,14 +1495,14 @@
         <v>52</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>388</v>
       </c>
@@ -1523,14 +1516,14 @@
         <v>53</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>388</v>
       </c>
@@ -1544,14 +1537,14 @@
         <v>54</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>388</v>
       </c>
@@ -1565,14 +1558,16 @@
         <v>55</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>389</v>
       </c>
@@ -1580,41 +1575,41 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>390</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>179</v>
+      <c r="C25" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>197</v>
+        <v>57</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>390</v>
       </c>
@@ -1622,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>58</v>
@@ -1631,181 +1626,181 @@
         <v>197</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>391</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>179</v>
+      <c r="C28" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="6" t="s">
         <v>189</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>62</v>
+        <v>178</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4.7</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>195</v>
+        <v>126</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>195</v>
+        <v>129</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>196</v>
+        <v>130</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>393</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D34" s="4">
-        <v>4.7</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>127</v>
+      <c r="C34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>393</v>
       </c>
@@ -1813,20 +1808,20 @@
         <v>9</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>393</v>
       </c>
@@ -1834,188 +1829,190 @@
         <v>9</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>132</v>
+        <v>10</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D40" s="6"/>
+        <v>178</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E40" s="3" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>179</v>
+        <v>12</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>184</v>
+        <v>76</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>185</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>396</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>179</v>
+      <c r="C44" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>204</v>
+        <v>79</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>396</v>
       </c>
@@ -2023,316 +2020,316 @@
         <v>12</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>145</v>
+        <v>13</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>397</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D50" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>398</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>399</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G50" s="6"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="6">
-        <v>397</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="6">
-        <v>397</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F52" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>180</v>
+        <v>16</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4.12</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="3" t="s">
-        <v>200</v>
+        <v>16</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>179</v>
+        <v>16</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>201</v>
+        <v>108</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>202</v>
+        <v>136</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>401</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D59" s="4">
-        <v>4.12</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>168</v>
+      <c r="C59" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>401</v>
       </c>
@@ -2340,484 +2337,360 @@
         <v>16</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>135</v>
+        <v>17</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="4">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>404</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E64" s="6" t="s">
+      <c r="D65" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="F64" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="6">
-        <v>401</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>180</v>
-      </c>
       <c r="F65" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="3" t="s">
-        <v>168</v>
+        <v>19</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>179</v>
+        <v>19</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>193</v>
+        <v>117</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C68" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>404</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>405</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D70" s="4">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>405</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>405</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>405</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>405</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>406</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="6">
-        <v>403</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G69" s="6"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="6">
-        <v>404</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70" s="4">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="6">
-        <v>404</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="6">
-        <v>404</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="6">
-        <v>404</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="6">
-        <v>404</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="6">
-        <v>404</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="D75" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D76" s="4">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>203</v>
+        <v>21</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="6">
-        <v>405</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G77" s="6"/>
-    </row>
-    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="6">
-        <v>405</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G78" s="6"/>
-    </row>
-    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="6">
-        <v>405</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G79" s="6"/>
-    </row>
-    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="6">
-        <v>406</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G80" s="6"/>
-    </row>
-    <row r="81" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="6">
-        <v>406</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G81" s="6"/>
-    </row>
-    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="6">
-        <v>406</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G82" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="G76" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Slicing algo: fixed the missing lasst slice
* The last H4 was getting missed due to unavailability of any further H4
to create an object for that slice:
** Added a flag to check if any H4 was found and for that added a slice
object at end of loop.
* Fixed the issue of processing invalid-questions (due to TypeError):
** try-except the TypeError for each question being processed.
* Improved the logging to console.
* Code cleanup.
</commit_message>
<xml_diff>
--- a/resources/section_mapping.xlsx
+++ b/resources/section_mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="205">
   <si>
     <t>Sections</t>
   </si>
@@ -469,9 +469,6 @@
   </si>
   <si>
     <t>&lt;&lt;$Shared Mailbox&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;$Distribution List and Shared Mailbox&gt;&gt; </t>
   </si>
   <si>
     <t>&lt;&lt;$Kerberos&gt;&gt;</t>
@@ -649,6 +646,9 @@
   </si>
   <si>
     <t>##NONE##</t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Distribution List and Shared Mailbox&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1060,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:A76"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,13 +1078,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -1093,10 +1093,10 @@
         <v>125</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1106,18 +1106,20 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="D2" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="3">
         <v>4.2</v>
@@ -1137,10 +1139,10 @@
         <v>128</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1151,16 +1153,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G4" s="6"/>
     </row>
@@ -1178,10 +1180,10 @@
         <v>33</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" s="6"/>
     </row>
@@ -1199,10 +1201,10 @@
         <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -1220,10 +1222,10 @@
         <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" s="6"/>
     </row>
@@ -1241,10 +1243,10 @@
         <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G8" s="6"/>
     </row>
@@ -1262,10 +1264,10 @@
         <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G9" s="6"/>
     </row>
@@ -1283,10 +1285,10 @@
         <v>38</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G10" s="6"/>
     </row>
@@ -1304,10 +1306,10 @@
         <v>39</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G11" s="6"/>
     </row>
@@ -1325,10 +1327,10 @@
         <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G12" s="6"/>
     </row>
@@ -1346,10 +1348,10 @@
         <v>41</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G13" s="6"/>
     </row>
@@ -1367,10 +1369,10 @@
         <v>42</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -1382,17 +1384,17 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="3" t="s">
         <v>128</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1403,7 +1405,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" s="3">
         <v>4.3</v>
@@ -1412,10 +1414,10 @@
         <v>127</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1432,10 +1434,10 @@
         <v>49</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G17" s="6"/>
     </row>
@@ -1453,10 +1455,10 @@
         <v>50</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G18" s="6"/>
     </row>
@@ -1474,10 +1476,10 @@
         <v>51</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G19" s="6"/>
     </row>
@@ -1495,10 +1497,10 @@
         <v>52</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G20" s="6"/>
     </row>
@@ -1516,10 +1518,10 @@
         <v>53</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G21" s="6"/>
     </row>
@@ -1537,10 +1539,10 @@
         <v>54</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G22" s="6"/>
     </row>
@@ -1561,10 +1563,10 @@
         <v>143</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1575,17 +1577,17 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1602,10 +1604,10 @@
         <v>57</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G25" s="6"/>
     </row>
@@ -1623,10 +1625,10 @@
         <v>58</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G26" s="6"/>
     </row>
@@ -1644,10 +1646,10 @@
         <v>59</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G27" s="6"/>
     </row>
@@ -1665,10 +1667,10 @@
         <v>60</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G28" s="6"/>
     </row>
@@ -1686,10 +1688,10 @@
         <v>61</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G29" s="6"/>
     </row>
@@ -1707,10 +1709,10 @@
         <v>62</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G30" s="6"/>
     </row>
@@ -1722,7 +1724,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="4">
         <v>4.7</v>
@@ -1731,10 +1733,10 @@
         <v>126</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1754,7 +1756,7 @@
         <v>129</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G32" s="6"/>
     </row>
@@ -1775,7 +1777,7 @@
         <v>130</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G33" s="6"/>
     </row>
@@ -1796,7 +1798,7 @@
         <v>131</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G34" s="6"/>
     </row>
@@ -1817,7 +1819,7 @@
         <v>132</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G35" s="6"/>
     </row>
@@ -1835,10 +1837,10 @@
         <v>71</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G36" s="6"/>
     </row>
@@ -1850,17 +1852,17 @@
         <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="3" t="s">
         <v>126</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1877,10 +1879,10 @@
         <v>74</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G38" s="6"/>
     </row>
@@ -1898,10 +1900,10 @@
         <v>75</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G39" s="6"/>
     </row>
@@ -1913,16 +1915,16 @@
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G40" s="6"/>
     </row>
@@ -1943,10 +1945,10 @@
         <v>143</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1966,7 +1968,7 @@
         <v>144</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G42" s="6"/>
     </row>
@@ -1984,10 +1986,10 @@
         <v>78</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G43" s="6"/>
     </row>
@@ -2008,7 +2010,7 @@
         <v>145</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -2029,7 +2031,7 @@
         <v>146</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G45" s="6"/>
     </row>
@@ -2041,16 +2043,16 @@
         <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" s="4">
         <v>4.0999999999999996</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -2068,10 +2070,10 @@
         <v>101</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G47" s="6"/>
     </row>
@@ -2089,10 +2091,10 @@
         <v>102</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G48" s="6"/>
     </row>
@@ -2110,10 +2112,10 @@
         <v>103</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G49" s="6"/>
     </row>
@@ -2131,10 +2133,10 @@
         <v>104</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G50" s="6"/>
     </row>
@@ -2146,17 +2148,17 @@
         <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2173,10 +2175,10 @@
         <v>105</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G52" s="6"/>
     </row>
@@ -2194,10 +2196,10 @@
         <v>106</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G53" s="6"/>
     </row>
@@ -2209,19 +2211,19 @@
         <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" s="4">
         <v>4.12</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2241,7 +2243,7 @@
         <v>133</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G55" s="6"/>
     </row>
@@ -2262,7 +2264,7 @@
         <v>134</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G56" s="6"/>
     </row>
@@ -2283,7 +2285,7 @@
         <v>135</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G57" s="6"/>
     </row>
@@ -2304,7 +2306,7 @@
         <v>136</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G58" s="6"/>
     </row>
@@ -2325,7 +2327,7 @@
         <v>137</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G59" s="6"/>
     </row>
@@ -2343,10 +2345,10 @@
         <v>112</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G60" s="6"/>
     </row>
@@ -2358,17 +2360,17 @@
         <v>17</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2385,10 +2387,10 @@
         <v>113</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G62" s="6"/>
     </row>
@@ -2406,10 +2408,10 @@
         <v>114</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G63" s="6"/>
     </row>
@@ -2421,19 +2423,19 @@
         <v>19</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D64" s="4">
         <v>4.1399999999999997</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2453,7 +2455,7 @@
         <v>138</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G65" s="6"/>
     </row>
@@ -2474,7 +2476,7 @@
         <v>139</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G66" s="6"/>
     </row>
@@ -2495,7 +2497,7 @@
         <v>140</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G67" s="6"/>
     </row>
@@ -2516,7 +2518,7 @@
         <v>141</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G68" s="6"/>
     </row>
@@ -2528,7 +2530,7 @@
         <v>19</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>119</v>
@@ -2537,7 +2539,7 @@
         <v>142</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G69" s="6"/>
     </row>
@@ -2549,19 +2551,19 @@
         <v>20</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D70" s="4">
         <v>4.1500000000000004</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2581,7 +2583,7 @@
         <v>147</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G71" s="6"/>
     </row>
@@ -2602,7 +2604,7 @@
         <v>148</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G72" s="6"/>
     </row>
@@ -2620,10 +2622,10 @@
         <v>122</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G73" s="6"/>
     </row>
@@ -2644,10 +2646,10 @@
         <v>143</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2664,10 +2666,10 @@
         <v>123</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G75" s="6"/>
     </row>
@@ -2685,10 +2687,10 @@
         <v>124</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G76" s="6"/>
     </row>

</xml_diff>

<commit_message>
Fixed issue of 'Other' as answers getting displayed always
* Introduced a new constant ##OTHER## in default field of
question-mapping.
* Renamed the <<$Other>> tags with detailed names: <<$Other_XYZ>>
* Removed the logic to add content of answers from linked questions in
bracket for Other as answer.
* Code cleanup.
</commit_message>
<xml_diff>
--- a/resources/section_mapping.xlsx
+++ b/resources/section_mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\DEV\PycharmProjects\application_questionnaire\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satyesha\PycharmProjects\application_questionnaire\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11565" tabRatio="453"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="11570" tabRatio="453"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="137">
   <si>
     <t>Specify if the application is known by any other name</t>
   </si>
@@ -195,12 +195,6 @@
     <t xml:space="preserve">&lt;&lt;$Forest_Domain_Name&gt;&gt;  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&lt;$Authetication_Mechanism&gt;&gt; </t>
-  </si>
-  <si>
-    <t>&lt;&lt;$Authetication_Type&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;&lt;$DMN1&gt;&gt; </t>
   </si>
   <si>
@@ -343,9 +337,6 @@
   </si>
   <si>
     <t>##QUESTION_DETAIL##</t>
-  </si>
-  <si>
-    <t>&lt;&lt;$Other&gt;&gt;</t>
   </si>
   <si>
     <t>&lt;&lt;APP_NAME&gt;&gt;</t>
@@ -408,9 +399,6 @@
     <t>Assessment Response</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&lt;$None_Authetication_Mechanism&gt;&gt; </t>
-  </si>
-  <si>
     <t>&lt;&lt;$None_File_and_Registry_Permissions&gt;&gt;</t>
   </si>
   <si>
@@ -424,6 +412,39 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Other_Authentication_Type&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Authentication_Type&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;$Authentication_Mechanism&gt;&gt; </t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Other_Authentication_Mechanism&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;$None_Authentication_Mechanism&gt;&gt; </t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Other_Forest_Domain_Name&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Other_Application_Access_Method&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;$Other_Host_Model&gt;&gt;</t>
+  </si>
+  <si>
+    <t>##ALL##,##OTHER##</t>
+  </si>
+  <si>
+    <t>##ALL##,##NONE##,##OTHER##</t>
+  </si>
+  <si>
+    <t>##OTHER##</t>
   </si>
 </sst>
 </file>
@@ -832,42 +853,42 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>385</v>
       </c>
@@ -875,19 +896,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>386</v>
       </c>
@@ -895,19 +916,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>386</v>
       </c>
@@ -915,17 +936,17 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>386</v>
       </c>
@@ -936,14 +957,14 @@
         <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>386</v>
       </c>
@@ -954,14 +975,14 @@
         <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>386</v>
       </c>
@@ -972,14 +993,14 @@
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>386</v>
       </c>
@@ -990,14 +1011,14 @@
         <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>386</v>
       </c>
@@ -1008,14 +1029,14 @@
         <v>21</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>386</v>
       </c>
@@ -1026,14 +1047,14 @@
         <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>386</v>
       </c>
@@ -1044,14 +1065,14 @@
         <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>386</v>
       </c>
@@ -1062,14 +1083,14 @@
         <v>24</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>386</v>
       </c>
@@ -1080,14 +1101,14 @@
         <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>386</v>
       </c>
@@ -1098,14 +1119,14 @@
         <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>387</v>
       </c>
@@ -1113,19 +1134,19 @@
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>388</v>
       </c>
@@ -1133,19 +1154,19 @@
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>388</v>
       </c>
@@ -1156,14 +1177,14 @@
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>388</v>
       </c>
@@ -1174,14 +1195,14 @@
         <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>388</v>
       </c>
@@ -1192,14 +1213,14 @@
         <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>388</v>
       </c>
@@ -1210,14 +1231,14 @@
         <v>29</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>388</v>
       </c>
@@ -1228,14 +1249,14 @@
         <v>30</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>388</v>
       </c>
@@ -1246,14 +1267,14 @@
         <v>25</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>388</v>
       </c>
@@ -1264,14 +1285,14 @@
         <v>31</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>389</v>
       </c>
@@ -1279,19 +1300,19 @@
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>392</v>
       </c>
@@ -1299,17 +1320,17 @@
         <v>5</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>392</v>
       </c>
@@ -1317,17 +1338,17 @@
         <v>5</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>393</v>
       </c>
@@ -1335,19 +1356,19 @@
         <v>6</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>393</v>
       </c>
@@ -1358,14 +1379,14 @@
         <v>32</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>393</v>
       </c>
@@ -1376,14 +1397,14 @@
         <v>33</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>393</v>
       </c>
@@ -1394,14 +1415,14 @@
         <v>34</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>393</v>
       </c>
@@ -1412,14 +1433,14 @@
         <v>35</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>393</v>
       </c>
@@ -1430,14 +1451,14 @@
         <v>25</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>394</v>
       </c>
@@ -1445,19 +1466,19 @@
         <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>396</v>
       </c>
@@ -1465,19 +1486,19 @@
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>396</v>
       </c>
@@ -1488,14 +1509,14 @@
         <v>31</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>396</v>
       </c>
@@ -1506,14 +1527,14 @@
         <v>36</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>396</v>
       </c>
@@ -1524,14 +1545,14 @@
         <v>37</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>396</v>
       </c>
@@ -1542,14 +1563,14 @@
         <v>38</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>396</v>
       </c>
@@ -1560,14 +1581,14 @@
         <v>39</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>397</v>
       </c>
@@ -1575,17 +1596,19 @@
         <v>9</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>397</v>
       </c>
@@ -1596,14 +1619,14 @@
         <v>40</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>397</v>
       </c>
@@ -1614,14 +1637,14 @@
         <v>41</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>397</v>
       </c>
@@ -1632,14 +1655,14 @@
         <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>397</v>
       </c>
@@ -1650,14 +1673,14 @@
         <v>25</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>398</v>
       </c>
@@ -1665,19 +1688,19 @@
         <v>10</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>401</v>
       </c>
@@ -1685,19 +1708,19 @@
         <v>11</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>401</v>
       </c>
@@ -1708,14 +1731,14 @@
         <v>43</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>401</v>
       </c>
@@ -1726,14 +1749,14 @@
         <v>44</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>401</v>
       </c>
@@ -1744,14 +1767,14 @@
         <v>45</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>401</v>
       </c>
@@ -1762,14 +1785,14 @@
         <v>46</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>401</v>
       </c>
@@ -1780,14 +1803,14 @@
         <v>47</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>401</v>
       </c>
@@ -1798,14 +1821,14 @@
         <v>25</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>402</v>
       </c>
@@ -1813,19 +1836,19 @@
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>403</v>
       </c>
@@ -1833,17 +1856,17 @@
         <v>13</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>403</v>
       </c>
@@ -1851,17 +1874,17 @@
         <v>13</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>404</v>
       </c>
@@ -1869,19 +1892,19 @@
         <v>14</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>404</v>
       </c>
@@ -1892,14 +1915,14 @@
         <v>48</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>404</v>
       </c>
@@ -1910,14 +1933,14 @@
         <v>49</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>404</v>
       </c>
@@ -1928,14 +1951,14 @@
         <v>50</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>404</v>
       </c>
@@ -1946,14 +1969,14 @@
         <v>51</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>404</v>
       </c>
@@ -1961,17 +1984,17 @@
         <v>14</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>405</v>
       </c>
@@ -1979,19 +2002,19 @@
         <v>15</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>405</v>
       </c>
@@ -2002,14 +2025,14 @@
         <v>52</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>405</v>
       </c>
@@ -2020,14 +2043,14 @@
         <v>53</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>405</v>
       </c>
@@ -2038,14 +2061,14 @@
         <v>54</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>405</v>
       </c>
@@ -2056,10 +2079,10 @@
         <v>31</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F66" s="5"/>
     </row>

</xml_diff>